<commit_message>
Modelo logico criado e dicionario de dados atualizado
</commit_message>
<xml_diff>
--- a/documents/DB/dicionario_dados.xlsx
+++ b/documents/DB/dicionario_dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Gabriel\Fatec\Fatec Sorocaba\7º Sem\MPTC\Trabalho\BaltaCompras\documents\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F453F2F8-62FE-41E2-933A-08F7C51046AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB33925E-7E97-43DB-B734-51E9A59C96AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="229">
   <si>
     <t>Requisicao</t>
   </si>
@@ -381,12 +381,6 @@
     <t>Transportadora</t>
   </si>
   <si>
-    <t>endereco</t>
-  </si>
-  <si>
-    <t>telefone</t>
-  </si>
-  <si>
     <t>MeioTransporte</t>
   </si>
   <si>
@@ -429,12 +423,6 @@
     <t>Ordem</t>
   </si>
   <si>
-    <t>Hexadecimal</t>
-  </si>
-  <si>
-    <t>Hash da senha do usuário</t>
-  </si>
-  <si>
     <t>Id da função do usuário</t>
   </si>
   <si>
@@ -498,9 +486,6 @@
     <t>Complemento</t>
   </si>
   <si>
-    <t>Alfabetico</t>
-  </si>
-  <si>
     <t>[A-Z][A-Z]</t>
   </si>
   <si>
@@ -703,6 +688,30 @@
   </si>
   <si>
     <t>Transportadora_MeioTransporte</t>
+  </si>
+  <si>
+    <t>Caracter</t>
+  </si>
+  <si>
+    <t>Hash da senha do usuário (Hexadecimal)</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Transportadora_Endereco</t>
+  </si>
+  <si>
+    <t>Transportadora_Email</t>
+  </si>
+  <si>
+    <t>Transportadora_Telefone</t>
+  </si>
+  <si>
+    <t>Char</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C98C66-8C7A-4082-8854-2BA6AF1B3236}">
   <dimension ref="B2:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1345,7 +1354,7 @@
         <v>255</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>13</v>
@@ -1354,7 +1363,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>135</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1374,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1405,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>13</v>
@@ -1414,7 +1423,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1472,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1492,7 +1501,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1550,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1570,7 +1579,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,10 +1634,10 @@
         <v>999999999</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,10 +1654,10 @@
         <v>999999999</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>6</v>
+        <v>223</v>
       </c>
       <c r="E26" s="11">
         <v>111</v>
@@ -1668,12 +1677,12 @@
         <v>13</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -1703,7 +1712,7 @@
     </row>
     <row r="30" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C30" s="11">
         <v>9</v>
@@ -1718,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1732,18 +1741,18 @@
         <v>12</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" s="11">
         <v>255</v>
@@ -1758,18 +1767,18 @@
         <v>13</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33" s="11">
         <v>8000</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>13</v>
@@ -1778,7 +1787,7 @@
         <v>13</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1795,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB871DF-4FEE-4096-9805-40D4A56FB639}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView showGridLines="0" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1870,7 +1879,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,7 +1900,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1912,16 +1921,16 @@
         <v>13</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7" s="11">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>18</v>
@@ -1933,16 +1942,16 @@
         <v>13</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="11">
-        <v>255</v>
+        <v>30</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>18</v>
@@ -1954,7 +1963,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
@@ -1975,7 +1984,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2037,7 +2046,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,7 +2109,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2121,7 +2130,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2175,10 +2184,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>13</v>
@@ -2240,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2261,7 +2270,7 @@
         <v>13</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="6" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,7 +2326,7 @@
         <v>7</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2332,13 +2341,13 @@
         <v>18</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2394,7 +2403,7 @@
         <v>45</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2415,7 +2424,7 @@
         <v>45</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2468,10 +2477,10 @@
         <v>999999999</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2489,10 +2498,10 @@
         <v>999999999</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,10 +2551,10 @@
         <v>999999999</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2563,10 +2572,10 @@
         <v>999999999</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2628,7 +2637,7 @@
         <v>7</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,7 +2658,7 @@
         <v>13</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2708,10 +2717,10 @@
         <v>999999999</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,10 +2738,10 @@
         <v>999999999</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2794,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2815,222 +2824,387 @@
         <v>13</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
-      <c r="B61" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C61" s="11">
-        <v>9</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="62" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="11">
-        <v>9</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>154</v>
-      </c>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
     </row>
     <row r="63" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="11">
-        <v>9</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>162</v>
+      <c r="B63" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
+      <c r="B64" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="11">
+        <v>9</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="25"/>
-    </row>
-    <row r="66" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="15" t="s">
+      <c r="B65" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="11">
+        <v>255</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="25"/>
+    </row>
+    <row r="68" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D68" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E68" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F66" s="17" t="s">
+      <c r="F68" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G66" s="16" t="s">
+      <c r="G68" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="18" t="s">
+    <row r="69" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C69" s="11">
+        <v>9</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C67" s="11">
-        <v>9</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F67" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C68" s="11">
-        <v>255</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="23" t="s">
+      <c r="C70" s="11">
+        <v>9</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="25"/>
-    </row>
-    <row r="71" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E71" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="18" t="s">
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="25"/>
+    </row>
+    <row r="73" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C72" s="11">
-        <v>9</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="G72" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C73" s="11">
-        <v>9</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="22">
-        <v>999999999</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>169</v>
+      <c r="C74" s="11">
+        <v>9</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75" s="11">
+        <v>9</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="25"/>
+    </row>
+    <row r="78" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G78" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" s="11">
+        <v>9</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="11">
+        <v>9</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="25"/>
+    </row>
+    <row r="83" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G83" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C84" s="11">
+        <v>9</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C85" s="11">
+        <v>9</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B65:G65"/>
+  <mergeCells count="15">
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B62:G62"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B2:G2"/>
@@ -3050,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G51"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView showGridLines="0" topLeftCell="B28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3112,7 +3286,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3126,7 +3300,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>13</v>
@@ -3192,7 +3366,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3203,7 +3377,7 @@
         <v>8000</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
@@ -3212,7 +3386,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3223,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>13</v>
@@ -3232,7 +3406,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3282,7 +3456,7 @@
         <v>7</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3302,7 +3476,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3322,12 +3496,12 @@
         <v>8</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C17" s="11">
         <v>2</v>
@@ -3342,7 +3516,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3389,10 +3563,10 @@
         <v>999999999</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3409,10 +3583,10 @@
         <v>999999999</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3432,7 +3606,7 @@
         <v>13</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3452,7 +3626,7 @@
         <v>13</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3472,7 +3646,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3562,7 +3736,7 @@
         <v>13</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3582,7 +3756,7 @@
         <v>13</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3699,7 +3873,7 @@
         <v>999999999</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>27</v>
@@ -3719,7 +3893,7 @@
         <v>999999999</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>10</v>
@@ -3742,10 +3916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CE2ABD-5051-4D6D-B9E2-AD0A024D9564}">
-  <dimension ref="A2:G47"/>
+  <dimension ref="A2:G46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3800,7 +3974,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3814,13 +3988,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3840,7 +4014,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3855,13 +4029,13 @@
         <v>47</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3873,7 +4047,7 @@
         <v>8000</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>13</v>
@@ -3882,7 +4056,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3894,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>13</v>
@@ -3903,7 +4077,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3915,48 +4089,59 @@
       <c r="F10" s="19"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
+    <row r="11" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>5</v>
+      <c r="B13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="11">
+        <v>9</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C14" s="11">
         <v>9</v>
@@ -3968,85 +4153,85 @@
         <v>999999999</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="22">
-        <v>999999999</v>
+        <v>22</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G15" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="11">
+        <v>9</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="11">
-        <v>8</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C20" s="11">
         <v>9</v>
@@ -4058,15 +4243,15 @@
         <v>999999999</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C21" s="11">
         <v>9</v>
@@ -4081,12 +4266,12 @@
         <v>8</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>191</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C22" s="11">
         <v>9</v>
@@ -4101,52 +4286,52 @@
         <v>8</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C23" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="22">
-        <v>999999999</v>
+        <v>47</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C24" s="11">
         <v>8</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>188</v>
+        <v>13</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="C25" s="11">
         <v>8</v>
@@ -4161,18 +4346,18 @@
         <v>13</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="C26" s="11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>13</v>
@@ -4181,82 +4366,82 @@
         <v>13</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="C27" s="11">
+        <v>8000</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="11">
-        <v>8000</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="25"/>
+      <c r="C30" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>5</v>
+      <c r="B31" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="11">
+        <v>9</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C32" s="11">
         <v>9</v>
@@ -4268,35 +4453,35 @@
         <v>999999999</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C33" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="22">
-        <v>999999999</v>
+        <v>22</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="11">
         <v>8</v>
@@ -4311,139 +4496,139 @@
         <v>13</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="11">
-        <v>8</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>206</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25"/>
+      <c r="B37" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>5</v>
+      <c r="B38" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="11">
+        <v>9</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="C39" s="11">
-        <v>9</v>
+        <v>255</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="22">
-        <v>999999999</v>
+        <v>18</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="11">
-        <v>255</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>208</v>
-      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="8"/>
+      <c r="B41" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="25"/>
+      <c r="B42" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>5</v>
+      <c r="B43" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="11">
+        <v>9</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="22">
+        <v>999999999</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C44" s="11">
         <v>9</v>
@@ -4455,41 +4640,41 @@
         <v>999999999</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C45" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="22">
-        <v>999999999</v>
+        <v>22</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="C46" s="11">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>22</v>
+        <v>224</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>13</v>
@@ -4498,37 +4683,17 @@
         <v>13</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="11">
-        <v>8000</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B41:G41"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4540,7 +4705,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4554,7 +4719,7 @@
     </row>
     <row r="3" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -4584,7 +4749,7 @@
     </row>
     <row r="5" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="11">
         <v>9</v>
@@ -4599,7 +4764,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4613,18 +4778,18 @@
         <v>12</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -4639,7 +4804,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4659,7 +4824,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4679,7 +4844,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4699,7 +4864,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4710,7 +4875,7 @@
         <v>8000</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>13</v>
@@ -4719,7 +4884,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4730,7 +4895,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>13</v>
@@ -4739,7 +4904,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -4755,8 +4920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408CC19B-9BBA-44ED-B36E-C6E708499583}">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4768,7 +4933,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -4798,7 +4963,7 @@
     </row>
     <row r="4" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C4" s="11">
         <v>9</v>
@@ -4813,7 +4978,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4827,13 +4992,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4873,7 +5038,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4884,7 +5049,7 @@
         <v>8000</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>13</v>
@@ -4893,7 +5058,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4904,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>13</v>
@@ -4913,7 +5078,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4925,18 +5090,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5112,6 +5277,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4738A93-B78B-4592-AE6C-7D4338D46FD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D28C32D-B13D-4D31-8555-6EE433CF36C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5123,14 +5296,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4738A93-B78B-4592-AE6C-7D4338D46FD2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>